<commit_message>
Remove blank lines from end of FY csv file
</commit_message>
<xml_diff>
--- a/InputData/plcy-schd/FY/FY Future Years.xlsx
+++ b/InputData/plcy-schd/FY/FY Future Years.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\plcy-schd\FY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\plcy-schd\FY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA21A683-9523-4DE0-9A38-94035A233DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A11848-89A1-46A2-AED1-E86E1643D610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{70679913-52CE-4866-92D3-04053F7F27F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{70679913-52CE-4866-92D3-04053F7F27F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6602441D-D56C-41AD-B87E-E90087615EB8}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -482,9 +482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA74B36-1D0A-45A2-9167-2B70446AECC4}">
   <dimension ref="A1:A100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Draft of generalized LCOE with future costs (#373)
</commit_message>
<xml_diff>
--- a/InputData/plcy-schd/FY/FY Future Years.xlsx
+++ b/InputData/plcy-schd/FY/FY Future Years.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\plcy-schd\FY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\plcy-schd\FY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A11848-89A1-46A2-AED1-E86E1643D610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EECE18C-C31E-4AD0-AED9-CFAACA9FC815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{70679913-52CE-4866-92D3-04053F7F27F8}"/>
+    <workbookView xWindow="60030" yWindow="3375" windowWidth="24075" windowHeight="13260" activeTab="2" xr2:uid="{70679913-52CE-4866-92D3-04053F7F27F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="FY" sheetId="2" r:id="rId2"/>
+    <sheet name="FFY" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>FY Future Years</t>
   </si>
@@ -52,6 +53,12 @@
   </si>
   <si>
     <t>FutureYear</t>
+  </si>
+  <si>
+    <t>Final Future Year</t>
+  </si>
+  <si>
+    <t>Final Time</t>
   </si>
 </sst>
 </file>
@@ -439,25 +446,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6602441D-D56C-41AD-B87E-E90087615EB8}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -465,12 +472,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>2021</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>2050</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -482,607 +497,635 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA74B36-1D0A-45A2-9167-2B70446AECC4}">
   <dimension ref="A1:A100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
         <f>"Year"&amp;About!A8</f>
         <v>Year2021</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f>IF(About!$A$8+ROW(A1)&gt;2100,"","Year"&amp;About!$A$8+ROW(A1))</f>
         <v>Year2022</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f>IF(About!$A$8+ROW(A2)&gt;2100,"","Year"&amp;About!$A$8+ROW(A2))</f>
         <v>Year2023</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>IF(About!$A$8+ROW(A3)&gt;2100,"","Year"&amp;About!$A$8+ROW(A3))</f>
         <v>Year2024</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f>IF(About!$A$8+ROW(A4)&gt;2100,"","Year"&amp;About!$A$8+ROW(A4))</f>
         <v>Year2025</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f>IF(About!$A$8+ROW(A5)&gt;2100,"","Year"&amp;About!$A$8+ROW(A5))</f>
         <v>Year2026</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
         <f>IF(About!$A$8+ROW(A6)&gt;2100,"","Year"&amp;About!$A$8+ROW(A6))</f>
         <v>Year2027</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f>IF(About!$A$8+ROW(A7)&gt;2100,"","Year"&amp;About!$A$8+ROW(A7))</f>
         <v>Year2028</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f>IF(About!$A$8+ROW(A8)&gt;2100,"","Year"&amp;About!$A$8+ROW(A8))</f>
         <v>Year2029</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f>IF(About!$A$8+ROW(A9)&gt;2100,"","Year"&amp;About!$A$8+ROW(A9))</f>
         <v>Year2030</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f>IF(About!$A$8+ROW(A10)&gt;2100,"","Year"&amp;About!$A$8+ROW(A10))</f>
         <v>Year2031</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f>IF(About!$A$8+ROW(A11)&gt;2100,"","Year"&amp;About!$A$8+ROW(A11))</f>
         <v>Year2032</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="str">
         <f>IF(About!$A$8+ROW(A12)&gt;2100,"","Year"&amp;About!$A$8+ROW(A12))</f>
         <v>Year2033</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="str">
         <f>IF(About!$A$8+ROW(A13)&gt;2100,"","Year"&amp;About!$A$8+ROW(A13))</f>
         <v>Year2034</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
         <f>IF(About!$A$8+ROW(A14)&gt;2100,"","Year"&amp;About!$A$8+ROW(A14))</f>
         <v>Year2035</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
         <f>IF(About!$A$8+ROW(A15)&gt;2100,"","Year"&amp;About!$A$8+ROW(A15))</f>
         <v>Year2036</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <f>IF(About!$A$8+ROW(A16)&gt;2100,"","Year"&amp;About!$A$8+ROW(A16))</f>
         <v>Year2037</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="str">
         <f>IF(About!$A$8+ROW(A17)&gt;2100,"","Year"&amp;About!$A$8+ROW(A17))</f>
         <v>Year2038</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="str">
         <f>IF(About!$A$8+ROW(A18)&gt;2100,"","Year"&amp;About!$A$8+ROW(A18))</f>
         <v>Year2039</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
         <f>IF(About!$A$8+ROW(A19)&gt;2100,"","Year"&amp;About!$A$8+ROW(A19))</f>
         <v>Year2040</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <f>IF(About!$A$8+ROW(A20)&gt;2100,"","Year"&amp;About!$A$8+ROW(A20))</f>
         <v>Year2041</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
         <f>IF(About!$A$8+ROW(A21)&gt;2100,"","Year"&amp;About!$A$8+ROW(A21))</f>
         <v>Year2042</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
         <f>IF(About!$A$8+ROW(A22)&gt;2100,"","Year"&amp;About!$A$8+ROW(A22))</f>
         <v>Year2043</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
         <f>IF(About!$A$8+ROW(A23)&gt;2100,"","Year"&amp;About!$A$8+ROW(A23))</f>
         <v>Year2044</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="str">
         <f>IF(About!$A$8+ROW(A24)&gt;2100,"","Year"&amp;About!$A$8+ROW(A24))</f>
         <v>Year2045</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="str">
         <f>IF(About!$A$8+ROW(A25)&gt;2100,"","Year"&amp;About!$A$8+ROW(A25))</f>
         <v>Year2046</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="str">
         <f>IF(About!$A$8+ROW(A26)&gt;2100,"","Year"&amp;About!$A$8+ROW(A26))</f>
         <v>Year2047</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="str">
         <f>IF(About!$A$8+ROW(A27)&gt;2100,"","Year"&amp;About!$A$8+ROW(A27))</f>
         <v>Year2048</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="str">
         <f>IF(About!$A$8+ROW(A28)&gt;2100,"","Year"&amp;About!$A$8+ROW(A28))</f>
         <v>Year2049</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
         <f>IF(About!$A$8+ROW(A29)&gt;2100,"","Year"&amp;About!$A$8+ROW(A29))</f>
         <v>Year2050</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
         <f>IF(About!$A$8+ROW(A30)&gt;2100,"","Year"&amp;About!$A$8+ROW(A30))</f>
         <v>Year2051</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="str">
         <f>IF(About!$A$8+ROW(A31)&gt;2100,"","Year"&amp;About!$A$8+ROW(A31))</f>
         <v>Year2052</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="str">
         <f>IF(About!$A$8+ROW(A32)&gt;2100,"","Year"&amp;About!$A$8+ROW(A32))</f>
         <v>Year2053</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="str">
         <f>IF(About!$A$8+ROW(A33)&gt;2100,"","Year"&amp;About!$A$8+ROW(A33))</f>
         <v>Year2054</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="str">
         <f>IF(About!$A$8+ROW(A34)&gt;2100,"","Year"&amp;About!$A$8+ROW(A34))</f>
         <v>Year2055</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="str">
         <f>IF(About!$A$8+ROW(A35)&gt;2100,"","Year"&amp;About!$A$8+ROW(A35))</f>
         <v>Year2056</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="str">
         <f>IF(About!$A$8+ROW(A36)&gt;2100,"","Year"&amp;About!$A$8+ROW(A36))</f>
         <v>Year2057</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="str">
         <f>IF(About!$A$8+ROW(A37)&gt;2100,"","Year"&amp;About!$A$8+ROW(A37))</f>
         <v>Year2058</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="str">
         <f>IF(About!$A$8+ROW(A38)&gt;2100,"","Year"&amp;About!$A$8+ROW(A38))</f>
         <v>Year2059</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="str">
         <f>IF(About!$A$8+ROW(A39)&gt;2100,"","Year"&amp;About!$A$8+ROW(A39))</f>
         <v>Year2060</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="str">
         <f>IF(About!$A$8+ROW(A40)&gt;2100,"","Year"&amp;About!$A$8+ROW(A40))</f>
         <v>Year2061</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="str">
         <f>IF(About!$A$8+ROW(A41)&gt;2100,"","Year"&amp;About!$A$8+ROW(A41))</f>
         <v>Year2062</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="str">
         <f>IF(About!$A$8+ROW(A42)&gt;2100,"","Year"&amp;About!$A$8+ROW(A42))</f>
         <v>Year2063</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="str">
         <f>IF(About!$A$8+ROW(A43)&gt;2100,"","Year"&amp;About!$A$8+ROW(A43))</f>
         <v>Year2064</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="str">
         <f>IF(About!$A$8+ROW(A44)&gt;2100,"","Year"&amp;About!$A$8+ROW(A44))</f>
         <v>Year2065</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="str">
         <f>IF(About!$A$8+ROW(A45)&gt;2100,"","Year"&amp;About!$A$8+ROW(A45))</f>
         <v>Year2066</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="str">
         <f>IF(About!$A$8+ROW(A46)&gt;2100,"","Year"&amp;About!$A$8+ROW(A46))</f>
         <v>Year2067</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="str">
         <f>IF(About!$A$8+ROW(A47)&gt;2100,"","Year"&amp;About!$A$8+ROW(A47))</f>
         <v>Year2068</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="str">
         <f>IF(About!$A$8+ROW(A48)&gt;2100,"","Year"&amp;About!$A$8+ROW(A48))</f>
         <v>Year2069</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="str">
         <f>IF(About!$A$8+ROW(A49)&gt;2100,"","Year"&amp;About!$A$8+ROW(A49))</f>
         <v>Year2070</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" t="str">
         <f>IF(About!$A$8+ROW(A50)&gt;2100,"","Year"&amp;About!$A$8+ROW(A50))</f>
         <v>Year2071</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" t="str">
         <f>IF(About!$A$8+ROW(A51)&gt;2100,"","Year"&amp;About!$A$8+ROW(A51))</f>
         <v>Year2072</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" t="str">
         <f>IF(About!$A$8+ROW(A52)&gt;2100,"","Year"&amp;About!$A$8+ROW(A52))</f>
         <v>Year2073</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" t="str">
         <f>IF(About!$A$8+ROW(A53)&gt;2100,"","Year"&amp;About!$A$8+ROW(A53))</f>
         <v>Year2074</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" t="str">
         <f>IF(About!$A$8+ROW(A54)&gt;2100,"","Year"&amp;About!$A$8+ROW(A54))</f>
         <v>Year2075</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" t="str">
         <f>IF(About!$A$8+ROW(A55)&gt;2100,"","Year"&amp;About!$A$8+ROW(A55))</f>
         <v>Year2076</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" t="str">
         <f>IF(About!$A$8+ROW(A56)&gt;2100,"","Year"&amp;About!$A$8+ROW(A56))</f>
         <v>Year2077</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" t="str">
         <f>IF(About!$A$8+ROW(A57)&gt;2100,"","Year"&amp;About!$A$8+ROW(A57))</f>
         <v>Year2078</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" t="str">
         <f>IF(About!$A$8+ROW(A58)&gt;2100,"","Year"&amp;About!$A$8+ROW(A58))</f>
         <v>Year2079</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" t="str">
         <f>IF(About!$A$8+ROW(A59)&gt;2100,"","Year"&amp;About!$A$8+ROW(A59))</f>
         <v>Year2080</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" t="str">
         <f>IF(About!$A$8+ROW(A60)&gt;2100,"","Year"&amp;About!$A$8+ROW(A60))</f>
         <v>Year2081</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" t="str">
         <f>IF(About!$A$8+ROW(A61)&gt;2100,"","Year"&amp;About!$A$8+ROW(A61))</f>
         <v>Year2082</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" t="str">
         <f>IF(About!$A$8+ROW(A62)&gt;2100,"","Year"&amp;About!$A$8+ROW(A62))</f>
         <v>Year2083</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" t="str">
         <f>IF(About!$A$8+ROW(A63)&gt;2100,"","Year"&amp;About!$A$8+ROW(A63))</f>
         <v>Year2084</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" t="str">
         <f>IF(About!$A$8+ROW(A64)&gt;2100,"","Year"&amp;About!$A$8+ROW(A64))</f>
         <v>Year2085</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" t="str">
         <f>IF(About!$A$8+ROW(A65)&gt;2100,"","Year"&amp;About!$A$8+ROW(A65))</f>
         <v>Year2086</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" t="str">
         <f>IF(About!$A$8+ROW(A66)&gt;2100,"","Year"&amp;About!$A$8+ROW(A66))</f>
         <v>Year2087</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" t="str">
         <f>IF(About!$A$8+ROW(A67)&gt;2100,"","Year"&amp;About!$A$8+ROW(A67))</f>
         <v>Year2088</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" t="str">
         <f>IF(About!$A$8+ROW(A68)&gt;2100,"","Year"&amp;About!$A$8+ROW(A68))</f>
         <v>Year2089</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" t="str">
         <f>IF(About!$A$8+ROW(A69)&gt;2100,"","Year"&amp;About!$A$8+ROW(A69))</f>
         <v>Year2090</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" t="str">
         <f>IF(About!$A$8+ROW(A70)&gt;2100,"","Year"&amp;About!$A$8+ROW(A70))</f>
         <v>Year2091</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" t="str">
         <f>IF(About!$A$8+ROW(A71)&gt;2100,"","Year"&amp;About!$A$8+ROW(A71))</f>
         <v>Year2092</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" t="str">
         <f>IF(About!$A$8+ROW(A72)&gt;2100,"","Year"&amp;About!$A$8+ROW(A72))</f>
         <v>Year2093</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" t="str">
         <f>IF(About!$A$8+ROW(A73)&gt;2100,"","Year"&amp;About!$A$8+ROW(A73))</f>
         <v>Year2094</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" t="str">
         <f>IF(About!$A$8+ROW(A74)&gt;2100,"","Year"&amp;About!$A$8+ROW(A74))</f>
         <v>Year2095</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" t="str">
         <f>IF(About!$A$8+ROW(A75)&gt;2100,"","Year"&amp;About!$A$8+ROW(A75))</f>
         <v>Year2096</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" t="str">
         <f>IF(About!$A$8+ROW(A76)&gt;2100,"","Year"&amp;About!$A$8+ROW(A76))</f>
         <v>Year2097</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" t="str">
         <f>IF(About!$A$8+ROW(A77)&gt;2100,"","Year"&amp;About!$A$8+ROW(A77))</f>
         <v>Year2098</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" t="str">
         <f>IF(About!$A$8+ROW(A78)&gt;2100,"","Year"&amp;About!$A$8+ROW(A78))</f>
         <v>Year2099</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" t="str">
         <f>IF(About!$A$8+ROW(A79)&gt;2100,"","Year"&amp;About!$A$8+ROW(A79))</f>
         <v>Year2100</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" t="str">
         <f>IF(About!$A$8+ROW(A80)&gt;2100,"","Year"&amp;About!$A$8+ROW(A80))</f>
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" t="str">
         <f>IF(About!$A$8+ROW(A81)&gt;2100,"","Year"&amp;About!$A$8+ROW(A81))</f>
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" t="str">
         <f>IF(About!$A$8+ROW(A82)&gt;2100,"","Year"&amp;About!$A$8+ROW(A82))</f>
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" t="str">
         <f>IF(About!$A$8+ROW(A83)&gt;2100,"","Year"&amp;About!$A$8+ROW(A83))</f>
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" t="str">
         <f>IF(About!$A$8+ROW(A84)&gt;2100,"","Year"&amp;About!$A$8+ROW(A84))</f>
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" t="str">
         <f>IF(About!$A$8+ROW(A85)&gt;2100,"","Year"&amp;About!$A$8+ROW(A85))</f>
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" t="str">
         <f>IF(About!$A$8+ROW(A86)&gt;2100,"","Year"&amp;About!$A$8+ROW(A86))</f>
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" t="str">
         <f>IF(About!$A$8+ROW(A87)&gt;2100,"","Year"&amp;About!$A$8+ROW(A87))</f>
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" t="str">
         <f>IF(About!$A$8+ROW(A88)&gt;2100,"","Year"&amp;About!$A$8+ROW(A88))</f>
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" t="str">
         <f>IF(About!$A$8+ROW(A89)&gt;2100,"","Year"&amp;About!$A$8+ROW(A89))</f>
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" t="str">
         <f>IF(About!$A$8+ROW(A90)&gt;2100,"","Year"&amp;About!$A$8+ROW(A90))</f>
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" t="str">
         <f>IF(About!$A$8+ROW(A91)&gt;2100,"","Year"&amp;About!$A$8+ROW(A91))</f>
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" t="str">
         <f>IF(About!$A$8+ROW(A92)&gt;2100,"","Year"&amp;About!$A$8+ROW(A92))</f>
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" t="str">
         <f>IF(About!$A$8+ROW(A93)&gt;2100,"","Year"&amp;About!$A$8+ROW(A93))</f>
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" t="str">
         <f>IF(About!$A$8+ROW(A94)&gt;2100,"","Year"&amp;About!$A$8+ROW(A94))</f>
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" t="str">
         <f>IF(About!$A$8+ROW(A95)&gt;2100,"","Year"&amp;About!$A$8+ROW(A95))</f>
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" t="str">
         <f>IF(About!$A$8+ROW(A96)&gt;2100,"","Year"&amp;About!$A$8+ROW(A96))</f>
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" t="str">
         <f>IF(About!$A$8+ROW(A97)&gt;2100,"","Year"&amp;About!$A$8+ROW(A97))</f>
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" t="str">
         <f>IF(About!$A$8+ROW(A98)&gt;2100,"","Year"&amp;About!$A$8+ROW(A98))</f>
         <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{168BBA54-9E73-41C3-81CD-077A74B6AB36}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="str">
+        <f>"Year"&amp;About!A9</f>
+        <v>Year2050</v>
       </c>
     </row>
   </sheetData>

</xml_diff>